<commit_message>
Execução do dia 21/10
</commit_message>
<xml_diff>
--- a/output/CodeSystem-AreaAtuacaoCodeSystem.xlsx
+++ b/output/CodeSystem-AreaAtuacaoCodeSystem.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://ehrruner.com/fhir/CodeSystem/AreaAtuacao</t>
+    <t>http://br-ipes.com/fhir/CodeSystem/AreaAtuacaoCodeSystem</t>
   </si>
   <si>
     <t>Version</t>
@@ -99,7 +99,7 @@
     <t>Value Set (all codes)</t>
   </si>
   <si>
-    <t>http://ehrruner.com/fhir/StructureDefinition/ValueSet/AreaAtuacao</t>
+    <t>http://br-ipes.com/fhir/StructureDefinition/ValueSet/AreaAtuacao</t>
   </si>
   <si>
     <t>Hierarchy</t>

</xml_diff>